<commit_message>
Add updated output CSVs and code changes for signal filters
</commit_message>
<xml_diff>
--- a/data_ref/NSE_Stocks.xlsx
+++ b/data_ref/NSE_Stocks.xlsx
@@ -3444,7 +3444,7 @@
     <t>DATA PATTERNS INDIA LTD</t>
   </si>
   <si>
-    <t>NSE_EQ|INE045601015</t>
+    <t>NSE_EQ|INE045601023</t>
   </si>
   <si>
     <t>PARAS</t>
@@ -18231,7 +18231,7 @@
       </c>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="A360" s="1" t="s">
+      <c r="A360" s="2" t="s">
         <v>1142</v>
       </c>
       <c r="B360" s="1" t="s">

</xml_diff>